<commit_message>
done half of Workshop
</commit_message>
<xml_diff>
--- a/מעקב תרגילים.xlsx
+++ b/מעקב תרגילים.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="50">
   <si>
     <t>שבוע 1</t>
   </si>
@@ -4197,7 +4197,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="23.1" customHeight="1"/>
@@ -4628,13 +4628,13 @@
         <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="13" t="str">
         <f ca="1">IF(AND(NOT(ISBLANK(F16)), NOT(F16 = "לא ניתן תרגיל")), IF(OR(F18 = "כן", F18 = "לא"), "", F16-TODAY()), "")</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="13">
+        <v/>
+      </c>
+      <c r="G17" s="13" t="str">
         <f ca="1">IF(AND(NOT(ISBLANK(G16)), NOT(G16 = "לא ניתן תרגיל")), IF(OR(G18 = "כן", G18 = "לא"), "", G16-TODAY()), "")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H17" s="13">
         <f t="shared" ca="1" si="10"/>
@@ -4651,8 +4651,12 @@
       <c r="E18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="F18" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="17.399999999999999" customHeight="1">
@@ -4674,11 +4678,11 @@
       </c>
       <c r="F19" s="29" t="str">
         <f>IF(F18 = "כן","בוצע", IF(F18 = "לא", "לא הוגש", IF((F16 = "לא ניתן תרגיל"), "", IF(NOT(ISBLANK(F16)), "טרם", ""))))</f>
-        <v>טרם</v>
+        <v>בוצע</v>
       </c>
       <c r="G19" s="29" t="str">
         <f>IF(G18 = "כן","בוצע", IF(G18 = "לא", "לא הוגש", IF((G16 = "לא ניתן תרגיל"), "", IF(NOT(ISBLANK(G16)), "טרם", ""))))</f>
-        <v>טרם</v>
+        <v>בוצע</v>
       </c>
       <c r="H19" s="29" t="str">
         <f t="shared" si="11"/>
@@ -8199,6 +8203,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="A30:A34"/>
     <mergeCell ref="A60:A64"/>
     <mergeCell ref="A65:A69"/>
     <mergeCell ref="A70:A74"/>
@@ -8207,11 +8216,6 @@
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="A30:A34"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:F5">
     <cfRule type="containsText" dxfId="370" priority="208" operator="containsText" text="לא הוגש">
@@ -10730,6 +10734,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A62:A66"/>
     <mergeCell ref="A32:A36"/>
@@ -10738,11 +10747,6 @@
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:F5">
     <cfRule type="containsText" dxfId="168" priority="215" operator="containsText" text="לא הוגש">

</xml_diff>

<commit_message>
Started Ex4 in fnc prog
</commit_message>
<xml_diff>
--- a/מעקב תרגילים.xlsx
+++ b/מעקב תרגילים.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="52">
   <si>
     <t>שבוע 1</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>לא רלוונטי</t>
+  </si>
+  <si>
+    <t>לא</t>
   </si>
 </sst>
 </file>
@@ -4124,7 +4127,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="23.1" customHeight="1"/>
@@ -4570,13 +4573,11 @@
         <f>IF(D16 = "לא ניתן תרגיל", "לא ניתן תרגיל", "")</f>
         <v/>
       </c>
-      <c r="E20" s="32" t="str">
-        <f>IF(E16 = "לא ניתן תרגיל", "לא ניתן תרגיל", "")</f>
-        <v/>
-      </c>
-      <c r="F20" s="32" t="str">
-        <f>IF(F16 = "לא ניתן תרגיל", "לא ניתן תרגיל", "")</f>
-        <v/>
+      <c r="E20" s="32">
+        <v>100</v>
+      </c>
+      <c r="F20" s="32">
+        <v>100</v>
       </c>
       <c r="G20" s="32" t="str">
         <f>IF(G16 = "לא ניתן תרגיל", "לא ניתן תרגיל", "")</f>
@@ -4702,19 +4703,19 @@
       </c>
       <c r="C26" s="13">
         <f t="shared" ref="C26" ca="1" si="15">IF(AND(NOT(ISBLANK(C25)), NOT(C25 = "לא ניתן תרגיל")), IF(OR(C27 = "כן", C27 = "לא"), "", C25-TODAY()), "")</f>
-        <v>8</v>
-      </c>
-      <c r="D26" s="13">
+        <v>7</v>
+      </c>
+      <c r="D26" s="13" t="str">
         <f ca="1">IF(AND(NOT(ISBLANK(D25)), NOT(D25 = "לא ניתן תרגיל")), IF(OR(D27 = "כן", D27 = "לא"), "", D25-TODAY()), "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E26" s="13">
         <f ca="1">IF(AND(NOT(ISBLANK(E25)), NOT(E25 = "לא ניתן תרגיל")), IF(OR(E27 = "כן", E27 = "לא"), "", E25-TODAY()), "")</f>
-        <v>5</v>
-      </c>
-      <c r="F26" s="13">
+        <v>4</v>
+      </c>
+      <c r="F26" s="13" t="str">
         <f ca="1">IF(AND(NOT(ISBLANK(F25)), NOT(F25 = "לא ניתן תרגיל")), IF(OR(F27 = "כן", F27 = "לא"), "", F25-TODAY()), "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G26" s="13" t="str">
         <f ca="1">IF(AND(NOT(ISBLANK(G25)), NOT(G25 = "לא ניתן תרגיל")), IF(OR(G27 = "כן", G27 = "לא"), "", G25-TODAY()), "")</f>
@@ -4727,9 +4728,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="F27" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" ht="17.399999999999999" customHeight="1">
@@ -4743,7 +4748,7 @@
       </c>
       <c r="D28" s="31" t="str">
         <f>IF(D27 = "כן","בוצע", IF(D27 = "לא", "לא הוגש", IF((D25 = "לא ניתן תרגיל"), "", IF(NOT(ISBLANK(D25)), "טרם", ""))))</f>
-        <v>טרם</v>
+        <v>בוצע</v>
       </c>
       <c r="E28" s="31" t="str">
         <f>IF(E27 = "כן","בוצע", IF(E27 = "לא", "לא הוגש", IF((E25 = "לא ניתן תרגיל"), "", IF(NOT(ISBLANK(E25)), "טרם", ""))))</f>
@@ -4751,7 +4756,7 @@
       </c>
       <c r="F28" s="31" t="str">
         <f>IF(F27 = "כן","בוצע", IF(F27 = "לא", "לא הוגש", IF((F25 = "לא ניתן תרגיל"), "", IF(NOT(ISBLANK(F25)), "טרם", ""))))</f>
-        <v>טרם</v>
+        <v>לא הוגש</v>
       </c>
       <c r="G28" s="31" t="str">
         <f>IF(G27 = "כן","בוצע", IF(G27 = "לא", "לא הוגש", IF((G25 = "לא ניתן תרגיל"), "", IF(NOT(ISBLANK(G25)), "טרם", ""))))</f>

</xml_diff>

<commit_message>
working on the last ip macro
</commit_message>
<xml_diff>
--- a/מעקב תרגילים.xlsx
+++ b/מעקב תרגילים.xlsx
@@ -4579,9 +4579,8 @@
       <c r="F20" s="32">
         <v>100</v>
       </c>
-      <c r="G20" s="32" t="str">
-        <f>IF(G16 = "לא ניתן תרגיל", "לא ניתן תרגיל", "")</f>
-        <v/>
+      <c r="G20" s="32">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17.399999999999999" hidden="1" customHeight="1">
@@ -4703,7 +4702,7 @@
       </c>
       <c r="C26" s="13">
         <f t="shared" ref="C26" ca="1" si="15">IF(AND(NOT(ISBLANK(C25)), NOT(C25 = "לא ניתן תרגיל")), IF(OR(C27 = "כן", C27 = "לא"), "", C25-TODAY()), "")</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D26" s="13" t="str">
         <f ca="1">IF(AND(NOT(ISBLANK(D25)), NOT(D25 = "לא ניתן תרגיל")), IF(OR(D27 = "כן", D27 = "לא"), "", D25-TODAY()), "")</f>
@@ -4711,7 +4710,7 @@
       </c>
       <c r="E26" s="13">
         <f ca="1">IF(AND(NOT(ISBLANK(E25)), NOT(E25 = "לא ניתן תרגיל")), IF(OR(E27 = "כן", E27 = "לא"), "", E25-TODAY()), "")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F26" s="13" t="str">
         <f ca="1">IF(AND(NOT(ISBLANK(F25)), NOT(F25 = "לא ניתן תרגיל")), IF(OR(F27 = "כן", F27 = "לא"), "", F25-TODAY()), "")</f>
@@ -7921,6 +7920,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="A30:A34"/>
     <mergeCell ref="A60:A64"/>
     <mergeCell ref="A65:A69"/>
     <mergeCell ref="A70:A74"/>
@@ -7929,11 +7933,6 @@
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="A30:A34"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:E5">
     <cfRule type="containsText" dxfId="357" priority="210" operator="containsText" text="לא הוגש">
@@ -10388,6 +10387,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A62:A66"/>
     <mergeCell ref="A32:A36"/>
@@ -10396,11 +10400,6 @@
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:F5">
     <cfRule type="containsText" dxfId="168" priority="215" operator="containsText" text="לא הוגש">

</xml_diff>